<commit_message>
Uploading Michael Phelps Graph.
</commit_message>
<xml_diff>
--- a/Final_Project/Source Data/Olympic Medal Count 2004 to 2012.xlsx
+++ b/Final_Project/Source Data/Olympic Medal Count 2004 to 2012.xlsx
@@ -7,21 +7,22 @@
     <workbookView xWindow="240" yWindow="120" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
   <sheets>
-    <sheet name="Total Medals Filtered (2)" sheetId="10" r:id="rId1"/>
-    <sheet name="Total Medals Filtered" sheetId="9" r:id="rId2"/>
-    <sheet name="Total Medals" sheetId="8" r:id="rId3"/>
-    <sheet name="Merged Table" sheetId="6" r:id="rId4"/>
-    <sheet name="Merged Table (2)" sheetId="7" r:id="rId5"/>
-    <sheet name="2012 Summer Olympic Medals" sheetId="2" r:id="rId6"/>
-    <sheet name="2008  Summer Olympics Medals" sheetId="4" r:id="rId7"/>
-    <sheet name="2004 Medal Count" sheetId="5" r:id="rId8"/>
+    <sheet name="Total Medals Transposed" sheetId="11" r:id="rId1"/>
+    <sheet name="Total Medals Filtered (2)" sheetId="10" r:id="rId2"/>
+    <sheet name="Total Medals Filtered" sheetId="9" r:id="rId3"/>
+    <sheet name="Total Medals" sheetId="8" r:id="rId4"/>
+    <sheet name="Merged Table" sheetId="6" r:id="rId5"/>
+    <sheet name="Merged Table (2)" sheetId="7" r:id="rId6"/>
+    <sheet name="2012 Summer Olympic Medals" sheetId="2" r:id="rId7"/>
+    <sheet name="2008  Summer Olympics Medals" sheetId="4" r:id="rId8"/>
+    <sheet name="2004 Medal Count" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="141">
   <si>
     <t>USA</t>
   </si>
@@ -367,6 +368,84 @@
   <si>
     <t>Michael Phelps</t>
   </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>North Korea</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Slovokia</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
 </sst>
 </file>
 
@@ -456,7 +535,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -697,11 +776,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="55"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="55"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -832,6 +924,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1127,13 +1234,639 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10" style="49" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A1" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A2" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="19">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="23">
+        <v>10</v>
+      </c>
+      <c r="F2" s="26">
+        <v>16</v>
+      </c>
+      <c r="G2" s="48">
+        <v>41803125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A3" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="19">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4">
+        <v>4</v>
+      </c>
+      <c r="E3" s="23">
+        <v>14</v>
+      </c>
+      <c r="F3" s="26">
+        <v>22</v>
+      </c>
+      <c r="G3" s="48">
+        <v>9514887</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A4" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="19">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4">
+        <v>15</v>
+      </c>
+      <c r="E4" s="23">
+        <v>20</v>
+      </c>
+      <c r="F4" s="26">
+        <v>43</v>
+      </c>
+      <c r="G4" s="48">
+        <v>9307609</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A5" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="19">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4">
+        <v>11</v>
+      </c>
+      <c r="E5" s="23">
+        <v>20</v>
+      </c>
+      <c r="F5" s="26">
+        <v>42</v>
+      </c>
+      <c r="G5" s="48">
+        <v>202033670</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A6" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="19">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3</v>
+      </c>
+      <c r="E6" s="23">
+        <v>13</v>
+      </c>
+      <c r="F6" s="26">
+        <v>19</v>
+      </c>
+      <c r="G6" s="48">
+        <v>7167998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A7" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="19">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4">
+        <v>9</v>
+      </c>
+      <c r="E7" s="23">
+        <v>8</v>
+      </c>
+      <c r="F7" s="26">
+        <v>25</v>
+      </c>
+      <c r="G7" s="48">
+        <v>10740468</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A8" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="19">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4">
+        <v>7</v>
+      </c>
+      <c r="E8" s="23">
+        <v>11</v>
+      </c>
+      <c r="F8" s="26">
+        <v>24</v>
+      </c>
+      <c r="G8" s="48">
+        <v>5640184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A9" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="19">
+        <v>9</v>
+      </c>
+      <c r="D9" s="4">
+        <v>5</v>
+      </c>
+      <c r="E9" s="23">
+        <v>7</v>
+      </c>
+      <c r="F9" s="26">
+        <v>21</v>
+      </c>
+      <c r="G9" s="48">
+        <v>96506031</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A10" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="19">
+        <v>6</v>
+      </c>
+      <c r="D10" s="4">
+        <v>5</v>
+      </c>
+      <c r="E10" s="23">
+        <v>6</v>
+      </c>
+      <c r="F10" s="26">
+        <v>17</v>
+      </c>
+      <c r="G10" s="48">
+        <v>4322842</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A11" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="19">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4">
+        <v>8</v>
+      </c>
+      <c r="E11" s="23">
+        <v>8</v>
+      </c>
+      <c r="F11" s="26">
+        <v>22</v>
+      </c>
+      <c r="G11" s="48">
+        <v>11128404</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A12" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="19">
+        <v>19</v>
+      </c>
+      <c r="D12" s="4">
+        <v>15</v>
+      </c>
+      <c r="E12" s="23">
+        <v>11</v>
+      </c>
+      <c r="F12" s="26">
+        <v>45</v>
+      </c>
+      <c r="G12" s="48">
+        <v>9933173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A13" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="19">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4">
+        <v>7</v>
+      </c>
+      <c r="E13" s="23">
+        <v>6</v>
+      </c>
+      <c r="F13" s="26">
+        <v>20</v>
+      </c>
+      <c r="G13" s="48">
+        <v>78470222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A14" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" s="19">
+        <v>12</v>
+      </c>
+      <c r="D14" s="4">
+        <v>8</v>
+      </c>
+      <c r="E14" s="23">
+        <v>8</v>
+      </c>
+      <c r="F14" s="26">
+        <v>28</v>
+      </c>
+      <c r="G14" s="49">
+        <v>2798837</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A15" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="19">
+        <v>10</v>
+      </c>
+      <c r="D15" s="4">
+        <v>9</v>
+      </c>
+      <c r="E15" s="23">
+        <v>15</v>
+      </c>
+      <c r="F15" s="26">
+        <v>34</v>
+      </c>
+      <c r="G15" s="49">
+        <v>16606878</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A16" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="19">
+        <v>9</v>
+      </c>
+      <c r="D16" s="4">
+        <v>12</v>
+      </c>
+      <c r="E16" s="23">
+        <v>11</v>
+      </c>
+      <c r="F16" s="26">
+        <v>32</v>
+      </c>
+      <c r="G16" s="49">
+        <v>45545980</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A17" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="19">
+        <v>18</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2</v>
+      </c>
+      <c r="E17" s="23">
+        <v>2</v>
+      </c>
+      <c r="F17" s="26">
+        <v>22</v>
+      </c>
+      <c r="G17" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A18" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="19">
+        <v>10</v>
+      </c>
+      <c r="D18" s="4">
+        <v>6</v>
+      </c>
+      <c r="E18" s="23">
+        <v>3</v>
+      </c>
+      <c r="F18" s="26">
+        <v>19</v>
+      </c>
+      <c r="G18" s="49">
+        <v>5091924</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A19" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="19">
+        <v>12</v>
+      </c>
+      <c r="D19" s="4">
+        <v>6</v>
+      </c>
+      <c r="E19" s="23">
+        <v>9</v>
+      </c>
+      <c r="F19" s="26">
+        <v>27</v>
+      </c>
+      <c r="G19" s="49">
+        <v>4551349</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A20" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="19">
+        <v>8</v>
+      </c>
+      <c r="D20" s="4">
+        <v>10</v>
+      </c>
+      <c r="E20" s="23">
+        <v>12</v>
+      </c>
+      <c r="F20" s="26">
+        <v>30</v>
+      </c>
+      <c r="G20" s="49">
+        <v>38220543</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A21" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="19">
+        <v>6</v>
+      </c>
+      <c r="D21" s="4">
+        <v>5</v>
+      </c>
+      <c r="E21" s="23">
+        <v>6</v>
+      </c>
+      <c r="F21" s="26">
+        <v>17</v>
+      </c>
+      <c r="G21" s="49">
+        <v>25026588</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A22" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="46" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="19">
+        <v>14</v>
+      </c>
+      <c r="D22" s="4">
+        <v>11</v>
+      </c>
+      <c r="E22" s="23">
+        <v>11</v>
+      </c>
+      <c r="F22" s="26">
+        <v>36</v>
+      </c>
+      <c r="G22" s="49">
+        <v>21640168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A23" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="C23" s="19">
+        <v>5</v>
+      </c>
+      <c r="D23" s="4">
+        <v>4</v>
+      </c>
+      <c r="E23" s="23">
+        <v>7</v>
+      </c>
+      <c r="F23" s="26">
+        <v>16</v>
+      </c>
+      <c r="G23" s="49">
+        <v>8157896</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A24" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="19">
+        <v>5</v>
+      </c>
+      <c r="D24" s="4">
+        <v>5</v>
+      </c>
+      <c r="E24" s="23">
+        <v>6</v>
+      </c>
+      <c r="F24" s="26">
+        <v>16</v>
+      </c>
+      <c r="G24" s="49">
+        <v>5454154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A25" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="19">
+        <v>5</v>
+      </c>
+      <c r="D25" s="4">
+        <v>10</v>
+      </c>
+      <c r="E25" s="23">
+        <v>5</v>
+      </c>
+      <c r="F25" s="26">
+        <v>20</v>
+      </c>
+      <c r="G25" s="49">
+        <v>9631261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="13.5" thickBot="1">
+      <c r="A26" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="19">
+        <v>6</v>
+      </c>
+      <c r="D26" s="4">
+        <v>10</v>
+      </c>
+      <c r="E26" s="23">
+        <v>8</v>
+      </c>
+      <c r="F26" s="26">
+        <v>24</v>
+      </c>
+      <c r="G26" s="49">
+        <v>75837020</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:F26">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1590,7 +2323,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -2068,7 +2801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E107"/>
   <sheetViews>
@@ -3910,7 +4643,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P107"/>
   <sheetViews>
@@ -9367,7 +10100,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA110"/>
   <sheetViews>
@@ -18802,7 +19535,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S101"/>
   <sheetViews>
@@ -24407,7 +25140,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D87"/>
   <sheetViews>
@@ -25647,7 +26380,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D76"/>
   <sheetViews>

</xml_diff>

<commit_message>
Uploading the webpage to Github for serving in a project directory.
</commit_message>
<xml_diff>
--- a/Final_Project/Source Data/Olympic Medal Count 2004 to 2012.xlsx
+++ b/Final_Project/Source Data/Olympic Medal Count 2004 to 2012.xlsx
@@ -1240,7 +1240,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1638,9 +1638,7 @@
       <c r="F17" s="26">
         <v>22</v>
       </c>
-      <c r="G17" s="48">
-        <v>1</v>
-      </c>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1">
       <c r="A18" s="26" t="s">

</xml_diff>